<commit_message>
doc: 2020-03-12 공부한 내용 추가
</commit_message>
<xml_diff>
--- a/exmaples/spring/teachers/portfolio URL매핑정책.xlsx
+++ b/exmaples/spring/teachers/portfolio URL매핑정책.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12885" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14190" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="memberDAO IF" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="230">
   <si>
     <t>기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -747,16 +747,181 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/board/modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BoardSVC.modify</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>BoardDAO.modify
 BoardDAO.fileModify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글답글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board/reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board/modify{bnum}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/board/reply/{bnum}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardSVC.reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardDAO.reply
+BoardDAO.fileModify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글답글(양식)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>replyFrom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bnum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글목록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rboard/{page}/{bnum}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardSVC.list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardDAO.list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rboard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardVO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardSVC.write</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardDAO.write</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardSVC.modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardDAO.modify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rboard/{rnum}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rnum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardSVC.delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardDAO.delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대댓글작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rboard/reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardSVC.reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardDAO.reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선호/비선호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rboard/vote</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VoteVO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardSVC.mergeVote</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RboardDAO.mergeVote</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AJAX Call</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page, bnum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2486,21 +2651,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.375" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2546,7 +2711,7 @@
         <v>156</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -2568,7 +2733,7 @@
       <c r="G3" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2592,7 +2757,7 @@
       <c r="G4" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" s="7" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -2616,7 +2781,7 @@
       <c r="G5" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -2638,11 +2803,11 @@
       <c r="G6" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>181</v>
       </c>
@@ -2664,14 +2829,14 @@
       <c r="G7" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>179</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>173</v>
@@ -2681,36 +2846,64 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2721,44 +2914,160 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>228</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>